<commit_message>
-se documenta mejor readme.README.md
-se crea un ejemplo de uso para control directo
-se crean dos funciones para posicionar el servo segun el valor de un potenciometro
</commit_message>
<xml_diff>
--- a/Calculos posicion y ADC.xlsx
+++ b/Calculos posicion y ADC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\SynologyDrive\IDEAA Lab\Proyectos\Controlador de servos RF\Firmware\ControladorServosRF.X\servo_library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4294CF-9498-4CEF-A5F5-EA45C154603B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A63F2-19CB-4DFB-8C01-E03C821E744A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41865" yWindow="3600" windowWidth="23970" windowHeight="11490" activeTab="1" xr2:uid="{7592B63C-CEEC-464A-9F40-153DC77A53F9}"/>
+    <workbookView xWindow="3720" yWindow="3315" windowWidth="23970" windowHeight="11490" activeTab="1" xr2:uid="{7592B63C-CEEC-464A-9F40-153DC77A53F9}"/>
   </bookViews>
   <sheets>
     <sheet name="254" sheetId="1" r:id="rId1"/>
@@ -12248,7 +12248,7 @@
   <dimension ref="B1:O264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12487,7 +12487,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>$I$2+ROUNDDOWN(($B9*$I$4)/256,0)</f>
         <v>507</v>
       </c>
       <c r="J9">

</xml_diff>